<commit_message>
refactoring to remove warnings
</commit_message>
<xml_diff>
--- a/MatchRunner/calibration.xlsx
+++ b/MatchRunner/calibration.xlsx
@@ -9,13 +9,6 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="pFour">Sheet1!$F$4</definedName>
-    <definedName name="pOut">Sheet1!$F$2</definedName>
-    <definedName name="pSingle">Sheet1!$F$6</definedName>
-    <definedName name="pSix">Sheet1!$F$3</definedName>
-    <definedName name="pTwo">Sheet1!$F$5</definedName>
-  </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
@@ -473,7 +466,7 @@
   <dimension ref="C2:AF47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+      <selection activeCell="E6" sqref="E6:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -599,8 +592,20 @@
     </row>
     <row r="6" spans="3:32">
       <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
+      <c r="E6" s="11">
+        <f t="array" ref="E6:F6">LINEST(F3:F5,E3:E5)</f>
+        <v>-0.3385806906137836</v>
+      </c>
+      <c r="F6" s="11">
+        <v>1.2912319515980082</v>
+      </c>
+      <c r="G6" s="11">
+        <f t="array" ref="G6:H6">LINEST(H3:H5,G3:G5)</f>
+        <v>-0.31393867323536934</v>
+      </c>
+      <c r="H6" s="11">
+        <v>1.190680766726125</v>
+      </c>
       <c r="M6" s="4"/>
     </row>
     <row r="8" spans="3:32">

</xml_diff>